<commit_message>
determined pdf fitting is worse than standard IDPT cross-correlation-based localization.
</commit_message>
<xml_diff>
--- a/publication/results/fit_plane/idpt_cm0.5_bin-r_rmse-z.xlsx
+++ b/publication/results/fit_plane/idpt_cm0.5_bin-r_rmse-z.xlsx
@@ -493,28 +493,28 @@
         <v>109.4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9573673704756551</v>
+        <v>0.957367370475656</v>
       </c>
       <c r="D2" t="n">
         <v>2.889159891598922</v>
       </c>
       <c r="E2" t="n">
-        <v>77.37882478219105</v>
+        <v>77.37882478217249</v>
       </c>
       <c r="F2" t="n">
-        <v>3.18731362354337</v>
+        <v>3.187313698723376</v>
       </c>
       <c r="G2" t="n">
-        <v>0.007267676184587893</v>
+        <v>0.007267960210422842</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2353475726795492</v>
+        <v>0.2353476541135442</v>
       </c>
       <c r="I2" t="n">
-        <v>123.8061196515057</v>
+        <v>123.806119651476</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3461627608315733</v>
+        <v>0.3461628232694998</v>
       </c>
       <c r="K2" t="n">
         <v>738</v>
@@ -528,28 +528,28 @@
         <v>215.9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.957216341542907</v>
+        <v>0.9572163415429076</v>
       </c>
       <c r="D3" t="n">
         <v>2.645650372825192</v>
       </c>
       <c r="E3" t="n">
-        <v>139.1824612391227</v>
+        <v>139.1824612391096</v>
       </c>
       <c r="F3" t="n">
-        <v>2.876779590905812</v>
+        <v>2.876779682491797</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.03983099537116672</v>
+        <v>-0.03983069453188608</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2693624698542336</v>
+        <v>0.2693625045091764</v>
       </c>
       <c r="I3" t="n">
-        <v>222.6919379825964</v>
+        <v>222.6919379825754</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4194721339516554</v>
+        <v>0.4194721768534259</v>
       </c>
       <c r="K3" t="n">
         <v>1207</v>
@@ -563,28 +563,28 @@
         <v>322.4</v>
       </c>
       <c r="C4" t="n">
-        <v>0.958904573979285</v>
+        <v>0.9589045739792855</v>
       </c>
       <c r="D4" t="n">
         <v>2.534755463059319</v>
       </c>
       <c r="E4" t="n">
-        <v>206.0695631132288</v>
+        <v>206.0695631132143</v>
       </c>
       <c r="F4" t="n">
-        <v>2.829815733905383</v>
+        <v>2.829815756760742</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02425181691175134</v>
+        <v>0.02425204723864799</v>
       </c>
       <c r="H4" t="n">
-        <v>0.247351022489034</v>
+        <v>0.2473510967298287</v>
       </c>
       <c r="I4" t="n">
-        <v>329.7113009811661</v>
+        <v>329.7113009811429</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3669137113166842</v>
+        <v>0.366913746353614</v>
       </c>
       <c r="K4" t="n">
         <v>1922</v>
@@ -598,28 +598,28 @@
         <v>428.9</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9515494493280764</v>
+        <v>0.9515494493280773</v>
       </c>
       <c r="D5" t="n">
         <v>2.070593013809916</v>
       </c>
       <c r="E5" t="n">
-        <v>259.3467258830917</v>
+        <v>259.3467258830887</v>
       </c>
       <c r="F5" t="n">
-        <v>2.302948962984184</v>
+        <v>2.302949523011714</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.003799151821184979</v>
+        <v>-0.003798389796727079</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2840702936407691</v>
+        <v>0.2840700369580191</v>
       </c>
       <c r="I5" t="n">
-        <v>414.9547614129468</v>
+        <v>414.9547614129419</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4173164915760085</v>
+        <v>0.4173163711173047</v>
       </c>
       <c r="K5" t="n">
         <v>1231</v>

</xml_diff>